<commit_message>
Updates to the conf file
</commit_message>
<xml_diff>
--- a/prob_calculator.xlsx
+++ b/prob_calculator.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5240" yWindow="7500" windowWidth="38400" windowHeight="22600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>c499</t>
   </si>
@@ -563,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -667,15 +668,15 @@
         <v>0.45</v>
       </c>
       <c r="H4" s="4">
-        <f>2/E4</f>
+        <f t="shared" ref="H4:J5" si="0">2/E4</f>
         <v>17.777777777777779</v>
       </c>
       <c r="I4" s="4">
-        <f>2/F4</f>
+        <f t="shared" si="0"/>
         <v>8.8888888888888893</v>
       </c>
       <c r="J4" s="4">
-        <f>2/G4</f>
+        <f t="shared" si="0"/>
         <v>4.4444444444444446</v>
       </c>
       <c r="K4" s="22">
@@ -683,11 +684,11 @@
         <v>18</v>
       </c>
       <c r="L4" s="22">
-        <f t="shared" ref="L4" si="0">ROUND(I4, 0)</f>
+        <f t="shared" ref="L4" si="1">ROUND(I4, 0)</f>
         <v>9</v>
       </c>
       <c r="M4" s="25">
-        <f t="shared" ref="M4" si="1">ROUND(J4, 0)</f>
+        <f t="shared" ref="M4" si="2">ROUND(J4, 0)</f>
         <v>4</v>
       </c>
     </row>
@@ -714,15 +715,15 @@
         <v>0.40594059405940597</v>
       </c>
       <c r="H5" s="4">
-        <f>2/E5</f>
+        <f t="shared" si="0"/>
         <v>19.707317073170731</v>
       </c>
       <c r="I5" s="4">
-        <f>2/F5</f>
+        <f t="shared" si="0"/>
         <v>9.8536585365853657</v>
       </c>
       <c r="J5" s="4">
-        <f>2/G5</f>
+        <f t="shared" si="0"/>
         <v>4.9268292682926829</v>
       </c>
       <c r="K5" s="9">
@@ -730,11 +731,11 @@
         <v>20</v>
       </c>
       <c r="L5" s="9">
-        <f t="shared" ref="K5:M7" si="2">ROUND(I5, 0)</f>
+        <f t="shared" ref="K5:M7" si="3">ROUND(I5, 0)</f>
         <v>10</v>
       </c>
       <c r="M5" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -765,23 +766,23 @@
         <v>25.533333333333331</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" ref="I6:I12" si="3">2/F6</f>
+        <f t="shared" ref="I6:I12" si="4">2/F6</f>
         <v>12.766666666666666</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" ref="J6:J12" si="4">2/G6</f>
+        <f t="shared" ref="J6:J12" si="5">2/G6</f>
         <v>6.3833333333333329</v>
       </c>
       <c r="K6" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="L6" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="M6" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
@@ -808,27 +809,27 @@
         <v>0.15018315018315018</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" ref="H7:H12" si="5">2/E7</f>
+        <f t="shared" ref="H7:H12" si="6">2/E7</f>
         <v>53.268292682926834</v>
       </c>
       <c r="I7" s="4">
+        <f t="shared" si="4"/>
+        <v>26.634146341463417</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="5"/>
+        <v>13.317073170731708</v>
+      </c>
+      <c r="K7" s="27">
         <f t="shared" si="3"/>
-        <v>26.634146341463417</v>
-      </c>
-      <c r="J7" s="4">
-        <f t="shared" si="4"/>
-        <v>13.317073170731708</v>
-      </c>
-      <c r="K7" s="27">
-        <f t="shared" si="2"/>
         <v>53</v>
       </c>
       <c r="L7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="M7" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
     </row>
@@ -859,23 +860,23 @@
         <v>69.019607843137251</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" ref="I8" si="6">2/F8</f>
+        <f t="shared" ref="I8" si="7">2/F8</f>
         <v>34.509803921568626</v>
       </c>
       <c r="J8" s="4">
-        <f t="shared" ref="J8" si="7">2/G8</f>
+        <f t="shared" ref="J8" si="8">2/G8</f>
         <v>76.688453159041401</v>
       </c>
       <c r="K8" s="9">
-        <f t="shared" ref="K8" si="8">ROUND(H8, 0)</f>
+        <f t="shared" ref="K8" si="9">ROUND(H8, 0)</f>
         <v>69</v>
       </c>
       <c r="L8" s="9">
-        <f t="shared" ref="L8" si="9">ROUND(I8, 0)</f>
+        <f t="shared" ref="L8" si="10">ROUND(I8, 0)</f>
         <v>35</v>
       </c>
       <c r="M8" s="10">
-        <f t="shared" ref="M8" si="10">ROUND(J8, 0)</f>
+        <f t="shared" ref="M8" si="11">ROUND(J8, 0)</f>
         <v>77</v>
       </c>
     </row>
@@ -902,27 +903,27 @@
         <v>0.26320201173512153</v>
       </c>
       <c r="H9" s="4">
+        <f t="shared" si="6"/>
+        <v>30.394904458598727</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="4"/>
+        <v>15.197452229299364</v>
+      </c>
+      <c r="J9" s="4">
         <f t="shared" si="5"/>
-        <v>30.394904458598727</v>
-      </c>
-      <c r="I9" s="4">
-        <f t="shared" si="3"/>
-        <v>15.197452229299364</v>
-      </c>
-      <c r="J9" s="4">
-        <f t="shared" si="4"/>
         <v>7.5987261146496818</v>
       </c>
       <c r="K9" s="22">
-        <f t="shared" ref="K9:K12" si="11">ROUND(H9, 0)</f>
+        <f t="shared" ref="K9:K12" si="12">ROUND(H9, 0)</f>
         <v>30</v>
       </c>
       <c r="L9" s="22">
-        <f t="shared" ref="L9:L12" si="12">ROUND(I9, 0)</f>
+        <f t="shared" ref="L9:L12" si="13">ROUND(I9, 0)</f>
         <v>15</v>
       </c>
       <c r="M9" s="25">
-        <f t="shared" ref="M9:M12" si="13">ROUND(J9, 0)</f>
+        <f t="shared" ref="M9:M12" si="14">ROUND(J9, 0)</f>
         <v>8</v>
       </c>
     </row>
@@ -949,27 +950,27 @@
         <v>4.4337926902336726E-2</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" ref="H10" si="14">2/E10</f>
+        <f t="shared" ref="H10" si="15">2/E10</f>
         <v>180.43243243243245</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" ref="I10" si="15">2/F10</f>
+        <f t="shared" ref="I10" si="16">2/F10</f>
         <v>90.216216216216225</v>
       </c>
       <c r="J10" s="4">
-        <f t="shared" ref="J10" si="16">2/G10</f>
+        <f t="shared" ref="J10" si="17">2/G10</f>
         <v>45.108108108108112</v>
       </c>
       <c r="K10" s="27">
-        <f t="shared" ref="K10" si="17">ROUND(H10, 0)</f>
+        <f t="shared" ref="K10" si="18">ROUND(H10, 0)</f>
         <v>180</v>
       </c>
       <c r="L10" s="27">
-        <f t="shared" ref="L10" si="18">ROUND(I10, 0)</f>
+        <f t="shared" ref="L10" si="19">ROUND(I10, 0)</f>
         <v>90</v>
       </c>
       <c r="M10" s="28">
-        <f t="shared" ref="M10" si="19">ROUND(J10, 0)</f>
+        <f t="shared" ref="M10" si="20">ROUND(J10, 0)</f>
         <v>45</v>
       </c>
     </row>
@@ -996,27 +997,27 @@
         <v>0.15431296055483312</v>
       </c>
       <c r="H11" s="4">
+        <f t="shared" si="6"/>
+        <v>51.842696629213478</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="4"/>
+        <v>25.921348314606739</v>
+      </c>
+      <c r="J11" s="4">
         <f t="shared" si="5"/>
-        <v>51.842696629213478</v>
-      </c>
-      <c r="I11" s="4">
-        <f t="shared" si="3"/>
-        <v>25.921348314606739</v>
-      </c>
-      <c r="J11" s="4">
-        <f t="shared" si="4"/>
         <v>12.960674157303369</v>
       </c>
       <c r="K11" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>52</v>
       </c>
       <c r="L11" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>26</v>
       </c>
       <c r="M11" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>13</v>
       </c>
     </row>
@@ -1043,27 +1044,27 @@
         <v>2.6490066225165563E-2</v>
       </c>
       <c r="H12" s="7">
+        <f t="shared" si="6"/>
+        <v>302</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="4"/>
+        <v>151</v>
+      </c>
+      <c r="J12" s="7">
         <f t="shared" si="5"/>
+        <v>75.5</v>
+      </c>
+      <c r="K12" s="23">
+        <f t="shared" si="12"/>
         <v>302</v>
       </c>
-      <c r="I12" s="7">
-        <f t="shared" si="3"/>
+      <c r="L12" s="23">
+        <f t="shared" si="13"/>
         <v>151</v>
       </c>
-      <c r="J12" s="7">
-        <f t="shared" si="4"/>
-        <v>75.5</v>
-      </c>
-      <c r="K12" s="23">
-        <f t="shared" si="11"/>
-        <v>302</v>
-      </c>
-      <c r="L12" s="23">
-        <f t="shared" si="12"/>
-        <v>151</v>
-      </c>
       <c r="M12" s="24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>76</v>
       </c>
     </row>
@@ -1119,4 +1120,145 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1">
+        <v>18</v>
+      </c>
+      <c r="C1">
+        <v>9</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>53</v>
+      </c>
+      <c r="C4">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>69</v>
+      </c>
+      <c r="C5">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>180</v>
+      </c>
+      <c r="C7">
+        <v>90</v>
+      </c>
+      <c r="D7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>52</v>
+      </c>
+      <c r="C8">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>302</v>
+      </c>
+      <c r="C9">
+        <v>151</v>
+      </c>
+      <c r="D9">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>